<commit_message>
three function not yet
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="163">
   <si>
     <t>AI、UQ、UN</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -790,12 +790,24 @@
     <t>Exp_Click_Sound ( 語音點擊紀錄 )</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>cs_click_time</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NN、ZF、UN</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ct_click_time</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1430,13 +1442,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H119" sqref="H119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="29.8984375" customWidth="1"/>
     <col min="2" max="2" width="36.8984375" customWidth="1"/>
@@ -1444,7 +1456,7 @@
     <col min="4" max="4" width="77.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="17">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>12</v>
@@ -1454,7 +1466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="17">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -1466,7 +1478,7 @@
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="17">
       <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
@@ -1478,7 +1490,7 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="17">
       <c r="A4" s="13" t="s">
         <v>17</v>
       </c>
@@ -1490,7 +1502,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="17">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>49</v>
@@ -1500,7 +1512,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="17">
       <c r="A8" s="3" t="s">
         <v>50</v>
       </c>
@@ -1512,7 +1524,7 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="17">
       <c r="A9" s="16" t="s">
         <v>104</v>
       </c>
@@ -1524,7 +1536,7 @@
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="17">
       <c r="A10" s="8" t="s">
         <v>105</v>
       </c>
@@ -1538,7 +1550,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="17">
       <c r="A11" s="5" t="s">
         <v>106</v>
       </c>
@@ -1552,7 +1564,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="17">
       <c r="A12" s="5" t="s">
         <v>138</v>
       </c>
@@ -1566,7 +1578,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="17">
       <c r="A13" s="21" t="s">
         <v>107</v>
       </c>
@@ -1580,7 +1592,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="17">
       <c r="A14" s="13" t="s">
         <v>102</v>
       </c>
@@ -1594,7 +1606,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="17">
       <c r="A15" s="13" t="s">
         <v>103</v>
       </c>
@@ -1608,7 +1620,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="17">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1620,7 +1632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="17">
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
@@ -1633,7 +1645,7 @@
       <c r="D19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="17">
       <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
@@ -1646,7 +1658,7 @@
       <c r="D20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="17">
       <c r="A21" s="26" t="s">
         <v>43</v>
       </c>
@@ -1660,7 +1672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="17">
       <c r="A22" s="24" t="s">
         <v>44</v>
       </c>
@@ -1674,7 +1686,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="17">
       <c r="A23" s="5" t="s">
         <v>59</v>
       </c>
@@ -1686,7 +1698,7 @@
       </c>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="17">
       <c r="A24" s="5" t="s">
         <v>60</v>
       </c>
@@ -1697,7 +1709,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="17">
       <c r="A25" s="16" t="s">
         <v>55</v>
       </c>
@@ -1708,7 +1720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="17">
       <c r="A26" s="16" t="s">
         <v>54</v>
       </c>
@@ -1719,13 +1731,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="17">
       <c r="A27" s="5"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="17">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>19</v>
@@ -1735,7 +1747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="17">
       <c r="A30" s="3" t="s">
         <v>32</v>
       </c>
@@ -1747,7 +1759,7 @@
       </c>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="17">
       <c r="A31" s="14" t="s">
         <v>22</v>
       </c>
@@ -1759,7 +1771,7 @@
       </c>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="17">
       <c r="A32" s="5" t="s">
         <v>33</v>
       </c>
@@ -1771,7 +1783,7 @@
       </c>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="17">
       <c r="A33" s="13" t="s">
         <v>34</v>
       </c>
@@ -1785,7 +1797,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="17">
       <c r="A34" s="5" t="s">
         <v>136</v>
       </c>
@@ -1799,7 +1811,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="17">
       <c r="A35" s="5" t="s">
         <v>137</v>
       </c>
@@ -1813,13 +1825,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="17">
       <c r="A36" s="5"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
     </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="17">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>46</v>
@@ -1829,7 +1841,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="17">
       <c r="A39" s="3" t="s">
         <v>47</v>
       </c>
@@ -1841,7 +1853,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="17">
       <c r="A40" s="14" t="s">
         <v>83</v>
       </c>
@@ -1853,7 +1865,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="17">
       <c r="A41" s="25" t="s">
         <v>48</v>
       </c>
@@ -1867,7 +1879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="17">
       <c r="A42" s="16" t="s">
         <v>141</v>
       </c>
@@ -1878,7 +1890,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="17">
       <c r="A43" s="5" t="s">
         <v>142</v>
       </c>
@@ -1889,7 +1901,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="17">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
         <v>87</v>
@@ -1899,7 +1911,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="17">
       <c r="A47" s="3" t="s">
         <v>88</v>
       </c>
@@ -1911,7 +1923,7 @@
       </c>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="17">
       <c r="A48" s="14" t="s">
         <v>89</v>
       </c>
@@ -1923,7 +1935,7 @@
       </c>
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="17">
       <c r="A49" s="27" t="s">
         <v>90</v>
       </c>
@@ -1937,7 +1949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="17">
       <c r="A50" s="16" t="s">
         <v>139</v>
       </c>
@@ -1948,7 +1960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="17">
       <c r="A51" s="5" t="s">
         <v>140</v>
       </c>
@@ -1959,7 +1971,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="17">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
         <v>62</v>
@@ -1969,7 +1981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="17">
       <c r="A55" s="3" t="s">
         <v>64</v>
       </c>
@@ -1981,7 +1993,7 @@
       </c>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="17">
       <c r="A56" s="13" t="s">
         <v>63</v>
       </c>
@@ -1993,7 +2005,7 @@
       </c>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="17">
       <c r="A57" s="23" t="s">
         <v>92</v>
       </c>
@@ -2005,16 +2017,16 @@
       </c>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="17">
       <c r="A58" s="13"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4">
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="17">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
         <v>66</v>
@@ -2024,7 +2036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="17">
       <c r="A61" s="3" t="s">
         <v>67</v>
       </c>
@@ -2036,7 +2048,7 @@
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="17">
       <c r="A62" s="13" t="s">
         <v>68</v>
       </c>
@@ -2048,7 +2060,7 @@
       </c>
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="17">
       <c r="A63" s="13" t="s">
         <v>93</v>
       </c>
@@ -2060,7 +2072,7 @@
       </c>
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="17">
       <c r="A64" s="21" t="s">
         <v>71</v>
       </c>
@@ -2071,7 +2083,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="17">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
         <v>69</v>
@@ -2081,7 +2093,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="17">
       <c r="A68" s="3" t="s">
         <v>75</v>
       </c>
@@ -2093,7 +2105,7 @@
       </c>
       <c r="D68" s="4"/>
     </row>
-    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="17">
       <c r="A69" s="13" t="s">
         <v>70</v>
       </c>
@@ -2105,7 +2117,7 @@
       </c>
       <c r="D69" s="4"/>
     </row>
-    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="17">
       <c r="A70" s="13" t="s">
         <v>94</v>
       </c>
@@ -2117,7 +2129,7 @@
       </c>
       <c r="D70" s="4"/>
     </row>
-    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="17">
       <c r="A71" s="13" t="s">
         <v>97</v>
       </c>
@@ -2129,7 +2141,7 @@
       </c>
       <c r="D71" s="4"/>
     </row>
-    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="17">
       <c r="A72" s="21" t="s">
         <v>98</v>
       </c>
@@ -2141,7 +2153,7 @@
       </c>
       <c r="D72" s="4"/>
     </row>
-    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="17">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
         <v>100</v>
@@ -2151,7 +2163,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="17">
       <c r="A76" s="3" t="s">
         <v>82</v>
       </c>
@@ -2163,7 +2175,7 @@
       </c>
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="17">
       <c r="A77" s="14" t="s">
         <v>76</v>
       </c>
@@ -2175,7 +2187,7 @@
       </c>
       <c r="D77" s="4"/>
     </row>
-    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="17">
       <c r="A78" s="21" t="s">
         <v>77</v>
       </c>
@@ -2189,7 +2201,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="17">
       <c r="A79" s="13" t="s">
         <v>95</v>
       </c>
@@ -2203,7 +2215,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="17">
       <c r="A80" s="13" t="s">
         <v>96</v>
       </c>
@@ -2217,7 +2229,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="17">
       <c r="A81" s="13" t="s">
         <v>61</v>
       </c>
@@ -2231,7 +2243,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="17">
       <c r="A82" s="5" t="s">
         <v>135</v>
       </c>
@@ -2242,7 +2254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="17">
       <c r="A85" s="1"/>
       <c r="B85" s="1" t="s">
         <v>159</v>
@@ -2252,7 +2264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="17">
       <c r="A86" s="3" t="s">
         <v>109</v>
       </c>
@@ -2264,7 +2276,7 @@
       </c>
       <c r="D86" s="4"/>
     </row>
-    <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="17">
       <c r="A87" s="14" t="s">
         <v>110</v>
       </c>
@@ -2276,7 +2288,7 @@
       </c>
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="17">
       <c r="A88" s="16" t="s">
         <v>114</v>
       </c>
@@ -2287,7 +2299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="17">
       <c r="A89" s="21" t="s">
         <v>111</v>
       </c>
@@ -2301,7 +2313,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="17">
       <c r="A90" s="13" t="s">
         <v>112</v>
       </c>
@@ -2315,7 +2327,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="17">
       <c r="A91" s="13" t="s">
         <v>113</v>
       </c>
@@ -2329,32 +2341,43 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="17">
       <c r="A92" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="17">
+      <c r="A93" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C93" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D92" s="19" t="s">
+      <c r="D93" s="19" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.3">
-      <c r="A93" s="5" t="s">
+    <row r="94" spans="1:4" ht="17">
+      <c r="A94" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C94" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="17">
       <c r="A96" s="1"/>
       <c r="B96" s="1" t="s">
         <v>122</v>
@@ -2364,7 +2387,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="17">
       <c r="A97" s="3" t="s">
         <v>146</v>
       </c>
@@ -2376,7 +2399,7 @@
       </c>
       <c r="D97" s="4"/>
     </row>
-    <row r="98" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="17">
       <c r="A98" s="14" t="s">
         <v>115</v>
       </c>
@@ -2388,7 +2411,7 @@
       </c>
       <c r="D98" s="4"/>
     </row>
-    <row r="99" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="17">
       <c r="A99" s="16" t="s">
         <v>116</v>
       </c>
@@ -2399,7 +2422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="17">
       <c r="A100" s="21" t="s">
         <v>147</v>
       </c>
@@ -2413,7 +2436,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="17">
       <c r="A101" s="13" t="s">
         <v>148</v>
       </c>
@@ -2427,7 +2450,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="17">
       <c r="A102" s="13" t="s">
         <v>149</v>
       </c>
@@ -2441,7 +2464,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="17">
       <c r="A103" s="13" t="s">
         <v>117</v>
       </c>
@@ -2455,7 +2478,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" ht="17">
       <c r="A104" s="5" t="s">
         <v>120</v>
       </c>
@@ -2466,7 +2489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="17">
       <c r="A107" s="1"/>
       <c r="B107" s="1" t="s">
         <v>150</v>
@@ -2476,7 +2499,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="17">
       <c r="A108" s="3" t="s">
         <v>123</v>
       </c>
@@ -2488,7 +2511,7 @@
       </c>
       <c r="D108" s="4"/>
     </row>
-    <row r="109" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="17">
       <c r="A109" s="14" t="s">
         <v>151</v>
       </c>
@@ -2500,7 +2523,7 @@
       </c>
       <c r="D109" s="4"/>
     </row>
-    <row r="110" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="17">
       <c r="A110" s="16" t="s">
         <v>124</v>
       </c>
@@ -2511,7 +2534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="17">
       <c r="A111" s="21" t="s">
         <v>125</v>
       </c>
@@ -2525,7 +2548,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="17">
       <c r="A112" s="13" t="s">
         <v>126</v>
       </c>
@@ -2539,7 +2562,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" ht="17">
       <c r="A113" s="13" t="s">
         <v>152</v>
       </c>
@@ -2553,7 +2576,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="17">
       <c r="A114" s="5" t="s">
         <v>127</v>
       </c>
@@ -2564,7 +2587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" ht="17">
       <c r="A118" s="1"/>
       <c r="B118" s="1" t="s">
         <v>158</v>
@@ -2574,7 +2597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" ht="17">
       <c r="A119" s="3" t="s">
         <v>153</v>
       </c>
@@ -2586,7 +2609,7 @@
       </c>
       <c r="D119" s="4"/>
     </row>
-    <row r="120" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" ht="17">
       <c r="A120" s="14" t="s">
         <v>128</v>
       </c>
@@ -2598,7 +2621,7 @@
       </c>
       <c r="D120" s="4"/>
     </row>
-    <row r="121" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" ht="17">
       <c r="A121" s="16" t="s">
         <v>129</v>
       </c>
@@ -2609,7 +2632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="17">
       <c r="A122" s="21" t="s">
         <v>130</v>
       </c>
@@ -2623,7 +2646,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="17">
       <c r="A123" s="13" t="s">
         <v>131</v>
       </c>
@@ -2637,7 +2660,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" ht="17">
       <c r="A124" s="13" t="s">
         <v>132</v>
       </c>
@@ -2651,7 +2674,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="17">
       <c r="A125" s="13" t="s">
         <v>143</v>
       </c>
@@ -2665,7 +2688,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" ht="17">
       <c r="A126" s="5" t="s">
         <v>133</v>
       </c>
@@ -2674,6 +2697,17 @@
       </c>
       <c r="C126" s="4" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="17">
+      <c r="A127" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>